<commit_message>
[Thermostat] Relé enclavament implementat (Yay!). SPIFlash bug fixed. OLED texts improved.
</commit_message>
<xml_diff>
--- a/sketches/Thermostat/schematic.xlsx
+++ b/sketches/Thermostat/schematic.xlsx
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>rst</t>
   </si>
@@ -190,9 +190,6 @@
     <t>ten</t>
   </si>
   <si>
-    <t>relé</t>
-  </si>
-  <si>
     <t>oled_vcc</t>
   </si>
   <si>
@@ -299,6 +296,12 @@
   </si>
   <si>
     <t>nc</t>
+  </si>
+  <si>
+    <t>relé+</t>
+  </si>
+  <si>
+    <t>relé-</t>
   </si>
 </sst>
 </file>
@@ -632,7 +635,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -671,9 +674,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -683,58 +683,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -770,24 +719,27 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -800,7 +752,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1914,7 +1911,7 @@
   <dimension ref="C1:AN31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="AY16" sqref="AY16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1927,73 +1924,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:40" s="13" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="37" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="2" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="27" t="s">
+      <c r="E2" s="54"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="27"/>
-      <c r="O2" s="28"/>
-      <c r="S2" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="45"/>
+      <c r="S2" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
     </row>
     <row r="3" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="41"/>
+        <v>40</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="54"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="14" t="s">
+      <c r="L3" s="24"/>
+      <c r="M3" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="S3" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="T3" s="48"/>
-      <c r="U3" s="48"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="S3" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
       <c r="AE3" s="7"/>
@@ -2009,124 +2006,126 @@
     </row>
     <row r="4" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="41"/>
+        <v>41</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="50"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="14" t="s">
+      <c r="L4" s="24"/>
+      <c r="M4" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
       <c r="AE4" s="7"/>
       <c r="AF4" s="7"/>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="16"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
+      <c r="AG4" s="15"/>
+      <c r="AH4" s="15"/>
+      <c r="AI4" s="15"/>
+      <c r="AJ4" s="15"/>
+      <c r="AK4" s="15"/>
+      <c r="AL4" s="15"/>
       <c r="AM4" s="7"/>
       <c r="AN4" s="7"/>
     </row>
     <row r="5" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="41"/>
+        <v>42</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="52"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="35" t="s">
+      <c r="L5" s="24"/>
+      <c r="M5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
       <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
       <c r="AF5" s="7"/>
-      <c r="AG5" s="16"/>
-      <c r="AH5" s="16"/>
-      <c r="AI5" s="16"/>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="16"/>
-      <c r="AL5" s="16"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
       <c r="AM5" s="7"/>
       <c r="AN5" s="7"/>
     </row>
     <row r="6" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="41"/>
+        <v>39</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="52"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="35" t="s">
+      <c r="L6" s="24"/>
+      <c r="M6" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
       <c r="S6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
       <c r="AF6" s="7"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="16"/>
-      <c r="AI6" s="16"/>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="16"/>
-      <c r="AL6" s="16"/>
+      <c r="AG6" s="15"/>
+      <c r="AH6" s="15"/>
+      <c r="AI6" s="15"/>
+      <c r="AJ6" s="15"/>
+      <c r="AK6" s="15"/>
+      <c r="AL6" s="15"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7"/>
     </row>
     <row r="7" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="41"/>
+        <v>43</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="50"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="19" t="s">
+      <c r="L7" s="24"/>
+      <c r="M7" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
       <c r="S7" s="2" t="s">
         <v>1</v>
       </c>
@@ -2134,35 +2133,35 @@
       <c r="AD7" s="7"/>
       <c r="AE7" s="7"/>
       <c r="AF7" s="7"/>
-      <c r="AG7" s="16"/>
-      <c r="AH7" s="16"/>
-      <c r="AI7" s="16"/>
-      <c r="AJ7" s="16"/>
-      <c r="AK7" s="16"/>
-      <c r="AL7" s="16"/>
+      <c r="AG7" s="15"/>
+      <c r="AH7" s="15"/>
+      <c r="AI7" s="15"/>
+      <c r="AJ7" s="15"/>
+      <c r="AK7" s="15"/>
+      <c r="AL7" s="15"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7"/>
     </row>
     <row r="8" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="41"/>
+        <v>44</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="52"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="19" t="s">
+      <c r="L8" s="24"/>
+      <c r="M8" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
       <c r="S8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2170,73 +2169,73 @@
       <c r="AD8" s="7"/>
       <c r="AE8" s="7"/>
       <c r="AF8" s="7"/>
-      <c r="AG8" s="16"/>
-      <c r="AH8" s="16"/>
-      <c r="AI8" s="16"/>
-      <c r="AJ8" s="16"/>
-      <c r="AK8" s="16"/>
-      <c r="AL8" s="16"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15"/>
+      <c r="AI8" s="15"/>
+      <c r="AJ8" s="15"/>
+      <c r="AK8" s="15"/>
+      <c r="AL8" s="15"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7"/>
     </row>
     <row r="9" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="41"/>
+        <v>45</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
       <c r="S9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
-      <c r="AF9" s="15"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="16"/>
-      <c r="AI9" s="16"/>
-      <c r="AJ9" s="16"/>
-      <c r="AK9" s="16"/>
-      <c r="AL9" s="16"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="15"/>
+      <c r="AH9" s="15"/>
+      <c r="AI9" s="15"/>
+      <c r="AJ9" s="15"/>
+      <c r="AK9" s="15"/>
+      <c r="AL9" s="15"/>
       <c r="AM9" s="7"/>
       <c r="AN9" s="7"/>
     </row>
     <row r="10" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="41"/>
+        <v>46</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="52"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="23"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
       <c r="S10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
@@ -2253,138 +2252,138 @@
     </row>
     <row r="11" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="41"/>
+        <v>47</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="19" t="s">
+      <c r="L11" s="24"/>
+      <c r="M11" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
       <c r="S11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
       <c r="AE11" s="7"/>
       <c r="AF11" s="7"/>
-      <c r="AG11" s="17"/>
-      <c r="AH11" s="17"/>
-      <c r="AI11" s="17"/>
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
-      <c r="AL11" s="17"/>
+      <c r="AG11" s="16"/>
+      <c r="AH11" s="16"/>
+      <c r="AI11" s="16"/>
+      <c r="AJ11" s="16"/>
+      <c r="AK11" s="16"/>
+      <c r="AL11" s="16"/>
       <c r="AM11" s="7"/>
       <c r="AN11" s="7"/>
     </row>
     <row r="12" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="41"/>
+        <v>48</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="K12" s="54"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="19" t="s">
+      <c r="J12" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="37"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
       <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
       <c r="AE12" s="7"/>
       <c r="AF12" s="7"/>
-      <c r="AG12" s="17"/>
-      <c r="AH12" s="17"/>
-      <c r="AI12" s="17"/>
-      <c r="AJ12" s="17"/>
-      <c r="AK12" s="17"/>
-      <c r="AL12" s="17"/>
+      <c r="AG12" s="16"/>
+      <c r="AH12" s="16"/>
+      <c r="AI12" s="16"/>
+      <c r="AJ12" s="16"/>
+      <c r="AK12" s="16"/>
+      <c r="AL12" s="16"/>
       <c r="AM12" s="7"/>
       <c r="AN12" s="7"/>
     </row>
     <row r="13" spans="3:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="41"/>
+        <v>49</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="19" t="s">
+      <c r="J13" s="38"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
       <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
       <c r="AE13" s="7"/>
       <c r="AF13" s="7"/>
-      <c r="AG13" s="17"/>
-      <c r="AH13" s="17"/>
-      <c r="AI13" s="17"/>
-      <c r="AJ13" s="17"/>
-      <c r="AK13" s="17"/>
-      <c r="AL13" s="17"/>
+      <c r="AG13" s="16"/>
+      <c r="AH13" s="16"/>
+      <c r="AI13" s="16"/>
+      <c r="AJ13" s="16"/>
+      <c r="AK13" s="16"/>
+      <c r="AL13" s="16"/>
       <c r="AM13" s="7"/>
       <c r="AN13" s="7"/>
     </row>
     <row r="14" spans="3:40" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
       <c r="AC14" s="7"/>
       <c r="AD14" s="7"/>
       <c r="AE14" s="7"/>
-      <c r="AF14" s="15"/>
-      <c r="AG14" s="17"/>
-      <c r="AH14" s="17"/>
-      <c r="AI14" s="17"/>
-      <c r="AJ14" s="17"/>
-      <c r="AK14" s="17"/>
-      <c r="AL14" s="17"/>
+      <c r="AF14" s="14"/>
+      <c r="AG14" s="16"/>
+      <c r="AH14" s="16"/>
+      <c r="AI14" s="16"/>
+      <c r="AJ14" s="16"/>
+      <c r="AK14" s="16"/>
+      <c r="AL14" s="16"/>
       <c r="AM14" s="7"/>
       <c r="AN14" s="7"/>
     </row>
@@ -2397,12 +2396,12 @@
       </c>
       <c r="AE16" s="3"/>
       <c r="AF16" s="7"/>
-      <c r="AG16" s="16"/>
-      <c r="AH16" s="16"/>
-      <c r="AI16" s="16"/>
-      <c r="AJ16" s="16"/>
-      <c r="AK16" s="16"/>
-      <c r="AL16" s="16"/>
+      <c r="AG16" s="15"/>
+      <c r="AH16" s="15"/>
+      <c r="AI16" s="15"/>
+      <c r="AJ16" s="15"/>
+      <c r="AK16" s="15"/>
+      <c r="AL16" s="15"/>
       <c r="AM16" s="3"/>
       <c r="AN16" s="3"/>
     </row>
@@ -2415,15 +2414,15 @@
       <c r="K17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="26"/>
+      <c r="L17" s="7"/>
       <c r="AE17" s="3"/>
       <c r="AF17" s="7"/>
-      <c r="AG17" s="16"/>
-      <c r="AH17" s="16"/>
-      <c r="AI17" s="16"/>
-      <c r="AJ17" s="17"/>
-      <c r="AK17" s="16"/>
-      <c r="AL17" s="16"/>
+      <c r="AG17" s="15"/>
+      <c r="AH17" s="15"/>
+      <c r="AI17" s="15"/>
+      <c r="AJ17" s="16"/>
+      <c r="AK17" s="15"/>
+      <c r="AL17" s="15"/>
       <c r="AM17" s="3"/>
       <c r="AN17" s="3"/>
     </row>
@@ -2431,30 +2430,30 @@
       <c r="G18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="46" t="s">
+      <c r="J18" s="28" t="s">
         <v>13</v>
       </c>
       <c r="AE18" s="3"/>
       <c r="AF18" s="7"/>
-      <c r="AG18" s="16"/>
+      <c r="AG18" s="15"/>
       <c r="AH18" s="7"/>
-      <c r="AI18" s="16"/>
-      <c r="AJ18" s="16"/>
-      <c r="AK18" s="52"/>
-      <c r="AL18" s="16"/>
+      <c r="AI18" s="15"/>
+      <c r="AJ18" s="15"/>
+      <c r="AK18" s="30"/>
+      <c r="AL18" s="15"/>
       <c r="AM18" s="3"/>
       <c r="AN18" s="3"/>
     </row>
     <row r="19" spans="4:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L19" s="2"/>
       <c r="AE19" s="3"/>
-      <c r="AF19" s="15"/>
-      <c r="AG19" s="16"/>
-      <c r="AH19" s="16"/>
-      <c r="AI19" s="16"/>
-      <c r="AJ19" s="16"/>
-      <c r="AK19" s="16"/>
-      <c r="AL19" s="16"/>
+      <c r="AF19" s="14"/>
+      <c r="AG19" s="15"/>
+      <c r="AH19" s="15"/>
+      <c r="AI19" s="15"/>
+      <c r="AJ19" s="15"/>
+      <c r="AK19" s="15"/>
+      <c r="AL19" s="15"/>
       <c r="AM19" s="3"/>
       <c r="AN19" s="3"/>
     </row>
@@ -2475,14 +2474,14 @@
       <c r="D21" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="29" t="s">
-        <v>20</v>
+      <c r="E21" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="F21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>1</v>
@@ -2506,18 +2505,18 @@
       <c r="AN21" s="3"/>
     </row>
     <row r="22" spans="4:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="J22" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
+      <c r="D22" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="J22" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
       <c r="AE22" s="3"/>
       <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
@@ -2530,10 +2529,10 @@
       <c r="AN22" s="3"/>
     </row>
     <row r="23" spans="4:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
       <c r="AE23" s="3"/>
       <c r="AF23" s="3"/>
       <c r="AG23" s="3"/>
@@ -2546,10 +2545,10 @@
       <c r="AN23" s="3"/>
     </row>
     <row r="24" spans="4:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
       <c r="AE24" s="3"/>
       <c r="AF24" s="3"/>
       <c r="AG24" s="3"/>
@@ -2647,6 +2646,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
     <mergeCell ref="D22:G24"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="S3:U3"/>
@@ -2663,21 +2677,6 @@
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="M7:O7"/>
     <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>